<commit_message>
Fix but with font, and rotation set at same time.
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/experimental08.xlsx
+++ b/t/regression/xlsx_files/experimental08.xlsx
@@ -167,16 +167,25 @@
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="47078016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:txPr>
-          <a:bodyPr rot="-2700000" vert="horz"/>
-          <a:lstStyle/>
-          <a:p/>
-        </c:txPr>
       </c:catAx>
       <c:valAx>
         <c:axId val="47078016"/>

</xml_diff>